<commit_message>
added more selections on the side
</commit_message>
<xml_diff>
--- a/data/data_dictionary_current.xlsx
+++ b/data/data_dictionary_current.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gpain/Documents/Work_Dashboards/Alaska/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gpain/Documents/Work_Dashboards/Virginia/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D3CAEB7-6CB4-B042-A696-4C9C545FC1A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A9BD809-D1F8-224A-9A60-EF4857ADA3D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40380" yWindow="500" windowWidth="41060" windowHeight="28300" activeTab="1" xr2:uid="{949A1E6F-A50E-0D47-B806-7BF7EBA35A5B}"/>
+    <workbookView xWindow="-38240" yWindow="660" windowWidth="18980" windowHeight="20800" activeTab="2" xr2:uid="{949A1E6F-A50E-0D47-B806-7BF7EBA35A5B}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="2" r:id="rId1"/>
@@ -43,7 +43,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{6A2B6172-D835-5049-8FF9-94BEE80D74AE}">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{4B8578A4-BB0B-0947-87E4-9D51F558A093}">
       <text>
         <r>
           <rPr>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1284" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1369" uniqueCount="423">
   <si>
     <t>table_name</t>
   </si>
@@ -1271,12 +1271,114 @@
   <si>
     <t>prgm_url</t>
   </si>
+  <si>
+    <t>Internal training provided for staff and/or board</t>
+  </si>
+  <si>
+    <t>Internal Training</t>
+  </si>
+  <si>
+    <t>External training provided by organization to community</t>
+  </si>
+  <si>
+    <t>External Training</t>
+  </si>
+  <si>
+    <t>Program or curriculum revision</t>
+  </si>
+  <si>
+    <t>Program Revision</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> In planning stages</t>
+  </si>
+  <si>
+    <t>In Planning Stages</t>
+  </si>
+  <si>
+    <t>New partnerships</t>
+  </si>
+  <si>
+    <t>New Partnerships</t>
+  </si>
+  <si>
+    <t>Staff or board diversification</t>
+  </si>
+  <si>
+    <t>Staff or Board Diversification</t>
+  </si>
+  <si>
+    <t>More inclusive marketing</t>
+  </si>
+  <si>
+    <t>More Inclusive Marketing</t>
+  </si>
+  <si>
+    <t>Classroom volunteers/presenters</t>
+  </si>
+  <si>
+    <t>Curriculum &amp; instructional materials</t>
+  </si>
+  <si>
+    <t>Field trips</t>
+  </si>
+  <si>
+    <t>Materials &amp; supplies</t>
+  </si>
+  <si>
+    <t>Materials &amp; Supplies</t>
+  </si>
+  <si>
+    <t>Events/Symposiums</t>
+  </si>
+  <si>
+    <t>Professional development/consulting for administrators</t>
+  </si>
+  <si>
+    <t>Professional Development for Admin</t>
+  </si>
+  <si>
+    <t>Professional development/consulting for teachers</t>
+  </si>
+  <si>
+    <t>Professional Development for Teachers</t>
+  </si>
+  <si>
+    <t>Supporting networks (online/in-person)</t>
+  </si>
+  <si>
+    <t>Supporting Networks (online/in-person)</t>
+  </si>
+  <si>
+    <t>Mobility/wheelchair accommodations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mobility </t>
+  </si>
+  <si>
+    <t>Special education accommodations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Special education </t>
+  </si>
+  <si>
+    <t>Deaf/hearing-impaired accommodations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deaf/hearing-impaired </t>
+  </si>
+  <si>
+    <t>Blind/sight-impaired accommodations</t>
+  </si>
+  <si>
+    <t>Blind/sight-impaired</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1349,6 +1451,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF112337"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1403,7 +1511,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1446,9 +1554,10 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2503,10 +2612,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09851FDF-4334-4E44-81EF-4155DEF57BA3}">
-  <dimension ref="A1:K123"/>
+  <dimension ref="A1:K122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A79" sqref="A79:XFD79"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3757,7 +3866,7 @@
         <v>13</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H21" s="2">
         <v>0</v>
@@ -3767,7 +3876,7 @@
         <v>0</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -3825,13 +3934,13 @@
         <v>14</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H23" s="2">
         <v>0</v>
       </c>
       <c r="J23" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K23" s="2" t="s">
         <v>13</v>
@@ -5598,26 +5707,46 @@
       </c>
     </row>
     <row r="79" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A79" s="2"/>
-      <c r="B79" s="20"/>
-      <c r="C79" s="2"/>
-      <c r="D79" s="2"/>
-      <c r="E79" s="2"/>
-      <c r="F79" s="2"/>
-      <c r="G79" s="2"/>
-      <c r="H79" s="2"/>
-      <c r="J79" s="2"/>
-      <c r="K79" s="2"/>
+      <c r="A79" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B79" s="14" t="s">
+        <v>279</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D79" s="2">
+        <v>9</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G79" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H79" s="2">
+        <v>0</v>
+      </c>
+      <c r="J79" s="2">
+        <v>3</v>
+      </c>
+      <c r="K79" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="80" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B80" s="14" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D80" s="4">
         <v>10</v>
@@ -5635,21 +5764,21 @@
         <v>0</v>
       </c>
       <c r="J80" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K80" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="81" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B81" s="14" t="s">
-        <v>280</v>
+        <v>260</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>38</v>
+        <v>354</v>
       </c>
       <c r="D81" s="2">
         <v>11</v>
@@ -5667,21 +5796,21 @@
         <v>0</v>
       </c>
       <c r="J81" s="2">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K81" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="82" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B82" s="14" t="s">
-        <v>260</v>
+      <c r="B82" s="2" t="s">
+        <v>261</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="D82" s="4">
         <v>12</v>
@@ -5709,11 +5838,11 @@
       <c r="A83" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B83" s="2" t="s">
-        <v>261</v>
+      <c r="B83" s="14" t="s">
+        <v>262</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="D83" s="2">
         <v>13</v>
@@ -5728,24 +5857,27 @@
         <v>14</v>
       </c>
       <c r="H83" s="2">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="I83" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="J83" s="2">
         <v>0</v>
       </c>
       <c r="K83" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="84" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B84" s="14" t="s">
-        <v>262</v>
+      <c r="B84" s="2" t="s">
+        <v>263</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="D84" s="4">
         <v>14</v>
@@ -5774,10 +5906,10 @@
         <v>30</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="D85" s="2">
         <v>15</v>
@@ -5806,10 +5938,10 @@
         <v>30</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="D86" s="4">
         <v>16</v>
@@ -5837,11 +5969,11 @@
       <c r="A87" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B87" s="2" t="s">
-        <v>269</v>
+      <c r="B87" s="14" t="s">
+        <v>266</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="D87" s="2">
         <v>17</v>
@@ -5869,11 +6001,11 @@
       <c r="A88" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B88" s="14" t="s">
-        <v>266</v>
+      <c r="B88" s="2" t="s">
+        <v>267</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="D88" s="4">
         <v>18</v>
@@ -5901,11 +6033,11 @@
       <c r="A89" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B89" s="2" t="s">
-        <v>267</v>
+      <c r="B89" s="14" t="s">
+        <v>270</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>361</v>
+        <v>36</v>
       </c>
       <c r="D89" s="2">
         <v>19</v>
@@ -5917,16 +6049,16 @@
         <v>13</v>
       </c>
       <c r="G89" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H89" s="2">
         <v>0</v>
       </c>
       <c r="J89" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K89" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="90" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5934,10 +6066,10 @@
         <v>30</v>
       </c>
       <c r="B90" s="14" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>36</v>
+        <v>362</v>
       </c>
       <c r="D90" s="4">
         <v>20</v>
@@ -5965,11 +6097,11 @@
       <c r="A91" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B91" s="14" t="s">
-        <v>271</v>
+      <c r="B91" s="2" t="s">
+        <v>272</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="D91" s="2">
         <v>21</v>
@@ -5998,10 +6130,10 @@
         <v>30</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="D92" s="4">
         <v>22</v>
@@ -6030,10 +6162,10 @@
         <v>30</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="D93" s="2">
         <v>23</v>
@@ -6062,10 +6194,10 @@
         <v>30</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="D94" s="4">
         <v>24</v>
@@ -6094,10 +6226,10 @@
         <v>30</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="C95" s="2" t="s">
-        <v>366</v>
+        <v>276</v>
+      </c>
+      <c r="C95" s="17" t="s">
+        <v>367</v>
       </c>
       <c r="D95" s="2">
         <v>25</v>
@@ -6126,10 +6258,10 @@
         <v>30</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="C96" s="17" t="s">
-        <v>367</v>
+        <v>277</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>368</v>
       </c>
       <c r="D96" s="4">
         <v>26</v>
@@ -6158,10 +6290,10 @@
         <v>30</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="D97" s="2">
         <v>27</v>
@@ -6190,10 +6322,10 @@
         <v>30</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="D98" s="4">
         <v>28</v>
@@ -6222,10 +6354,10 @@
         <v>30</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="D99" s="2">
         <v>29</v>
@@ -6254,10 +6386,10 @@
         <v>30</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="D100" s="4">
         <v>30</v>
@@ -6286,10 +6418,10 @@
         <v>30</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="D101" s="2">
         <v>31</v>
@@ -6318,10 +6450,10 @@
         <v>30</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>373</v>
+        <v>37</v>
       </c>
       <c r="D102" s="4">
         <v>32</v>
@@ -6350,10 +6482,10 @@
         <v>30</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>37</v>
+        <v>374</v>
       </c>
       <c r="D103" s="2">
         <v>33</v>
@@ -6381,11 +6513,11 @@
       <c r="A104" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B104" s="2" t="s">
-        <v>286</v>
+      <c r="B104" s="14" t="s">
+        <v>287</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="D104" s="4">
         <v>34</v>
@@ -6414,10 +6546,10 @@
         <v>30</v>
       </c>
       <c r="B105" s="14" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="D105" s="2">
         <v>35</v>
@@ -6446,10 +6578,10 @@
         <v>30</v>
       </c>
       <c r="B106" s="14" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="D106" s="4">
         <v>36</v>
@@ -6477,20 +6609,20 @@
       <c r="A107" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B107" s="14" t="s">
-        <v>289</v>
+      <c r="B107" s="2" t="s">
+        <v>290</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="D107" s="2">
         <v>37</v>
       </c>
       <c r="E107" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G107" s="2" t="s">
         <v>14</v>
@@ -6510,19 +6642,19 @@
         <v>30</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="D108" s="4">
         <v>38</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G108" s="2" t="s">
         <v>14</v>
@@ -6542,19 +6674,19 @@
         <v>30</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="D109" s="2">
         <v>39</v>
       </c>
       <c r="E109" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G109" s="2" t="s">
         <v>14</v>
@@ -6574,19 +6706,19 @@
         <v>30</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="D110" s="4">
         <v>40</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F110" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G110" s="2" t="s">
         <v>14</v>
@@ -6606,19 +6738,19 @@
         <v>30</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="D111" s="2">
         <v>41</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G111" s="2" t="s">
         <v>14</v>
@@ -6638,19 +6770,19 @@
         <v>30</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>382</v>
+        <v>96</v>
       </c>
       <c r="D112" s="4">
         <v>42</v>
       </c>
       <c r="E112" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G112" s="2" t="s">
         <v>14</v>
@@ -6670,19 +6802,19 @@
         <v>30</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>96</v>
+        <v>383</v>
       </c>
       <c r="D113" s="2">
         <v>43</v>
       </c>
       <c r="E113" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F113" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G113" s="2" t="s">
         <v>14</v>
@@ -6702,19 +6834,19 @@
         <v>30</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="D114" s="4">
         <v>44</v>
       </c>
       <c r="E114" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F114" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G114" s="2" t="s">
         <v>14</v>
@@ -6733,20 +6865,20 @@
       <c r="A115" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B115" s="2" t="s">
-        <v>297</v>
+      <c r="B115" s="18" t="s">
+        <v>298</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="D115" s="2">
         <v>45</v>
       </c>
       <c r="E115" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F115" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G115" s="2" t="s">
         <v>14</v>
@@ -6765,20 +6897,20 @@
       <c r="A116" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B116" s="18" t="s">
-        <v>298</v>
+      <c r="B116" s="2" t="s">
+        <v>299</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="D116" s="4">
         <v>46</v>
       </c>
       <c r="E116" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F116" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G116" s="2" t="s">
         <v>14</v>
@@ -6797,20 +6929,20 @@
       <c r="A117" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B117" s="2" t="s">
-        <v>299</v>
+      <c r="B117" s="18" t="s">
+        <v>300</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="D117" s="2">
         <v>47</v>
       </c>
       <c r="E117" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F117" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G117" s="2" t="s">
         <v>14</v>
@@ -6826,36 +6958,7 @@
       </c>
     </row>
     <row r="118" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B118" s="18" t="s">
-        <v>300</v>
-      </c>
-      <c r="C118" s="2" t="s">
-        <v>387</v>
-      </c>
-      <c r="D118" s="4">
-        <v>48</v>
-      </c>
-      <c r="E118" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F118" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G118" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H118" s="2">
-        <v>0</v>
-      </c>
-      <c r="J118" s="2">
-        <v>0</v>
-      </c>
-      <c r="K118" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="A118" s="2"/>
     </row>
     <row r="119" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="2"/>
@@ -6868,9 +6971,6 @@
     </row>
     <row r="122" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="2"/>
-    </row>
-    <row r="123" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A123" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6880,17 +6980,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D1373AD-CAFE-FC46-B12F-4E16ECB9F9F7}">
-  <dimension ref="A1:N94"/>
+  <dimension ref="A1:N115"/>
   <sheetViews>
-    <sheetView topLeftCell="A50" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B75" sqref="B75"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.6640625" customWidth="1"/>
-    <col min="4" max="4" width="35.1640625" customWidth="1"/>
+    <col min="3" max="3" width="43.1640625" customWidth="1"/>
+    <col min="4" max="4" width="44.33203125" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
     <col min="6" max="6" width="19.5" customWidth="1"/>
     <col min="7" max="7" width="28" customWidth="1"/>
@@ -8256,16 +8356,16 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>39</v>
+        <v>212</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>13</v>
+        <v>389</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>13</v>
+        <v>390</v>
       </c>
       <c r="E47" s="2">
         <v>1</v>
@@ -8273,230 +8373,226 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>39</v>
+        <v>212</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>14</v>
+        <v>391</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>14</v>
+        <v>392</v>
       </c>
       <c r="E48" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>272</v>
+        <v>212</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>132</v>
+        <v>393</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>132</v>
+        <v>394</v>
       </c>
       <c r="E49" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>272</v>
+        <v>212</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>133</v>
+        <v>395</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>133</v>
+        <v>396</v>
       </c>
       <c r="E50" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>272</v>
+        <v>212</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>134</v>
+        <v>397</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>134</v>
+        <v>398</v>
       </c>
       <c r="E51" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>272</v>
+        <v>212</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>135</v>
+        <v>399</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>135</v>
+        <v>400</v>
       </c>
       <c r="E52" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>272</v>
+        <v>212</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>136</v>
+        <v>401</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>136</v>
+        <v>402</v>
       </c>
       <c r="E53" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B54" s="14" t="s">
-        <v>264</v>
+      <c r="B54" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>137</v>
+        <v>13</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>137</v>
+        <v>13</v>
       </c>
       <c r="E54" s="2">
         <v>1</v>
       </c>
-      <c r="G54" s="2"/>
-      <c r="H54" s="2"/>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B55" s="14" t="s">
-        <v>264</v>
+      <c r="B55" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>138</v>
+        <v>14</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>138</v>
+        <v>14</v>
       </c>
       <c r="E55" s="2">
         <v>2</v>
       </c>
-      <c r="G55" s="2"/>
-      <c r="H55" s="2"/>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B56" s="14" t="s">
-        <v>264</v>
+      <c r="B56" s="2" t="s">
+        <v>272</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E56" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A57" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E57" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A58" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E58" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A57" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B57" s="14" t="s">
-        <v>264</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="E57" s="2">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="E59" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A58" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B58" s="14" t="s">
-        <v>264</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="E58" s="2">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="E60" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A59" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B59" s="14" t="s">
-        <v>264</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="E59" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A60" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B60" s="14" t="s">
-        <v>264</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="E60" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>30</v>
       </c>
@@ -8504,16 +8600,18 @@
         <v>264</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="E61" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="62" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="G61" s="2"/>
+      <c r="H61" s="2"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>30</v>
       </c>
@@ -8521,25 +8619,18 @@
         <v>264</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="E62" s="2">
-        <v>9</v>
-      </c>
-      <c r="F62" s="16"/>
+        <v>2</v>
+      </c>
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
-      <c r="I62" s="2"/>
-      <c r="J62" s="2"/>
-      <c r="K62" s="2"/>
-      <c r="L62" s="2"/>
-      <c r="M62" s="2"/>
-      <c r="N62" s="2"/>
-    </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>30</v>
       </c>
@@ -8547,16 +8638,16 @@
         <v>264</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="E63" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>30</v>
       </c>
@@ -8564,16 +8655,16 @@
         <v>264</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>146</v>
+        <v>96</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>146</v>
+        <v>96</v>
       </c>
       <c r="E64" s="2">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>30</v>
       </c>
@@ -8581,16 +8672,16 @@
         <v>264</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="E65" s="2">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
         <v>30</v>
       </c>
@@ -8598,16 +8689,16 @@
         <v>264</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="E66" s="2">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
         <v>30</v>
       </c>
@@ -8615,152 +8706,161 @@
         <v>264</v>
       </c>
       <c r="C67" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="E67" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A68" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B68" s="14" t="s">
+        <v>264</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E68" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B69" s="14" t="s">
+        <v>264</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E69" s="2">
+        <v>9</v>
+      </c>
+      <c r="F69" s="16"/>
+      <c r="G69" s="2"/>
+      <c r="H69" s="2"/>
+      <c r="I69" s="2"/>
+      <c r="J69" s="2"/>
+      <c r="K69" s="2"/>
+      <c r="L69" s="2"/>
+      <c r="M69" s="2"/>
+      <c r="N69" s="2"/>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A70" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B70" s="14" t="s">
+        <v>264</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E70" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A71" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B71" s="14" t="s">
+        <v>264</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E71" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A72" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B72" s="14" t="s">
+        <v>264</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E72" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A73" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B73" s="14" t="s">
+        <v>264</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E73" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A74" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B74" s="14" t="s">
+        <v>264</v>
+      </c>
+      <c r="C74" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D67" s="2" t="s">
+      <c r="D74" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="E67" s="2">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A68" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B68" s="14" t="s">
-        <v>270</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="D68" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="E68" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A69" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B69" s="14" t="s">
-        <v>270</v>
-      </c>
-      <c r="C69" s="17" t="s">
-        <v>150</v>
-      </c>
-      <c r="D69" s="17" t="s">
-        <v>150</v>
-      </c>
-      <c r="E69" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A70" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B70" s="14" t="s">
-        <v>270</v>
-      </c>
-      <c r="C70" s="17" t="s">
-        <v>151</v>
-      </c>
-      <c r="D70" s="17" t="s">
-        <v>152</v>
-      </c>
-      <c r="E70" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A71" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B71" s="14" t="s">
-        <v>270</v>
-      </c>
-      <c r="C71" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="D71" s="17" t="s">
-        <v>154</v>
-      </c>
-      <c r="E71" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A72" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B72" s="14" t="s">
-        <v>270</v>
-      </c>
-      <c r="C72" s="17" t="s">
-        <v>155</v>
-      </c>
-      <c r="D72" s="17" t="s">
-        <v>156</v>
-      </c>
-      <c r="E72" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A73" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B73" s="14" t="s">
-        <v>270</v>
-      </c>
-      <c r="C73" s="17" t="s">
-        <v>157</v>
-      </c>
-      <c r="D73" s="17" t="s">
-        <v>158</v>
-      </c>
-      <c r="E73" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A74" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B74" s="14" t="s">
-        <v>270</v>
-      </c>
-      <c r="C74" s="17" t="s">
-        <v>159</v>
-      </c>
-      <c r="D74" s="17" t="s">
-        <v>160</v>
-      </c>
       <c r="E74" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B75" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="C75" s="17" t="s">
-        <v>161</v>
-      </c>
-      <c r="D75" s="17" t="s">
-        <v>162</v>
+      <c r="C75" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="E75" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
         <v>30</v>
       </c>
@@ -8768,16 +8868,16 @@
         <v>270</v>
       </c>
       <c r="C76" s="17" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="D76" s="17" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="E76" s="2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
         <v>30</v>
       </c>
@@ -8785,16 +8885,16 @@
         <v>270</v>
       </c>
       <c r="C77" s="17" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
       <c r="D77" s="17" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="E77" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
         <v>30</v>
       </c>
@@ -8802,16 +8902,16 @@
         <v>270</v>
       </c>
       <c r="C78" s="17" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="D78" s="17" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="E78" s="2">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>30</v>
       </c>
@@ -8819,16 +8919,16 @@
         <v>270</v>
       </c>
       <c r="C79" s="17" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="D79" s="17" t="s">
-        <v>170</v>
+        <v>156</v>
       </c>
       <c r="E79" s="2">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
         <v>30</v>
       </c>
@@ -8836,13 +8936,13 @@
         <v>270</v>
       </c>
       <c r="C80" s="17" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
       <c r="D80" s="17" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="E80" s="2">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
@@ -8853,13 +8953,13 @@
         <v>270</v>
       </c>
       <c r="C81" s="17" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="D81" s="17" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="E81" s="2">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
@@ -8869,14 +8969,14 @@
       <c r="B82" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="C82" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="D82" s="2" t="s">
-        <v>175</v>
+      <c r="C82" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="D82" s="17" t="s">
+        <v>162</v>
       </c>
       <c r="E82" s="2">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
@@ -8886,14 +8986,14 @@
       <c r="B83" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="C83" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="D83" s="2" t="s">
-        <v>176</v>
+      <c r="C83" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="D83" s="17" t="s">
+        <v>164</v>
       </c>
       <c r="E83" s="2">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
@@ -8903,14 +9003,14 @@
       <c r="B84" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="C84" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="D84" s="2" t="s">
-        <v>177</v>
+      <c r="C84" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="D84" s="17" t="s">
+        <v>166</v>
       </c>
       <c r="E84" s="2">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
@@ -8920,14 +9020,14 @@
       <c r="B85" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="C85" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="D85" s="2" t="s">
-        <v>179</v>
+      <c r="C85" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="D85" s="17" t="s">
+        <v>168</v>
       </c>
       <c r="E85" s="2">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
@@ -8935,46 +9035,50 @@
         <v>30</v>
       </c>
       <c r="B86" s="14" t="s">
-        <v>279</v>
-      </c>
-      <c r="C86" t="s">
-        <v>180</v>
-      </c>
-      <c r="D86" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="E86" s="2"/>
+        <v>270</v>
+      </c>
+      <c r="C86" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="D86" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="E86" s="2">
+        <v>12</v>
+      </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B87" s="14" t="s">
-        <v>279</v>
-      </c>
-      <c r="C87" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="D87" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="E87" s="2"/>
+        <v>270</v>
+      </c>
+      <c r="C87" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="D87" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="E87" s="2">
+        <v>13</v>
+      </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B88" s="14" t="s">
-        <v>279</v>
-      </c>
-      <c r="C88" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="D88" s="2" t="s">
-        <v>183</v>
+        <v>270</v>
+      </c>
+      <c r="C88" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D88" s="17" t="s">
+        <v>174</v>
       </c>
       <c r="E88" s="2">
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
@@ -8982,16 +9086,16 @@
         <v>30</v>
       </c>
       <c r="B89" s="14" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="E89" s="2">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
@@ -8999,16 +9103,16 @@
         <v>30</v>
       </c>
       <c r="B90" s="14" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="E90" s="2">
-        <v>2</v>
+        <v>16</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
@@ -9016,16 +9120,16 @@
         <v>30</v>
       </c>
       <c r="B91" s="14" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="E91" s="2">
-        <v>3</v>
+        <v>17</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
@@ -9033,16 +9137,16 @@
         <v>30</v>
       </c>
       <c r="B92" s="14" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="E92" s="2">
-        <v>4</v>
+        <v>18</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
@@ -9050,16 +9154,16 @@
         <v>30</v>
       </c>
       <c r="B93" s="14" t="s">
-        <v>280</v>
-      </c>
-      <c r="C93" s="2" t="s">
-        <v>188</v>
+        <v>279</v>
+      </c>
+      <c r="C93" t="s">
+        <v>180</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="E93" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
@@ -9067,16 +9171,373 @@
         <v>30</v>
       </c>
       <c r="B94" s="14" t="s">
+        <v>279</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="E94" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A95" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B95" s="14" t="s">
+        <v>279</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="E95" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A96" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B96" s="14" t="s">
         <v>280</v>
       </c>
-      <c r="C94" s="2" t="s">
+      <c r="C96" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="E96" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A97" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B97" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="E97" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A98" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B98" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="E98" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A99" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B99" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="E99" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A100" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B100" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="E100" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A101" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B101" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="C101" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D94" s="2" t="s">
+      <c r="D101" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="E94" s="2">
+      <c r="E101" s="2">
         <v>6</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A102" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B102" s="20" t="s">
+        <v>260</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="E102" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A103" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B103" s="20" t="s">
+        <v>260</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="D103" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="E103" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A104" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B104" s="20" t="s">
+        <v>260</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="E104" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A105" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B105" s="20" t="s">
+        <v>260</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="E105" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A106" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B106" s="20" t="s">
+        <v>260</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="D106" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="E106" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A107" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B107" s="20" t="s">
+        <v>260</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="E107" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A108" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B108" s="20" t="s">
+        <v>260</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="E108" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A109" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B109" s="20" t="s">
+        <v>260</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="D109" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="E109" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A110" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B110" s="20" t="s">
+        <v>260</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="D110" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="E110" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A111" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B111" s="14" t="s">
+        <v>262</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="D111" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="E111" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A112" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B112" s="14" t="s">
+        <v>262</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="D112" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="E112" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A113" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B113" s="14" t="s">
+        <v>262</v>
+      </c>
+      <c r="C113" s="21" t="s">
+        <v>419</v>
+      </c>
+      <c r="D113" s="21" t="s">
+        <v>420</v>
+      </c>
+      <c r="E113" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A114" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B114" s="14" t="s">
+        <v>262</v>
+      </c>
+      <c r="C114" s="21" t="s">
+        <v>421</v>
+      </c>
+      <c r="D114" s="21" t="s">
+        <v>422</v>
+      </c>
+      <c r="E114" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A115" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B115" s="14" t="s">
+        <v>262</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D115" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E115" s="2">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added the new data and changed some fonts
</commit_message>
<xml_diff>
--- a/data/data_dictionary_current.xlsx
+++ b/data/data_dictionary_current.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gpain/Documents/Work_Dashboards/Virginia/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9BE4DDD-922A-B449-807A-1B4376406F2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D015716-88A7-874A-B87A-F5A612117493}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="760" windowWidth="29860" windowHeight="17240" activeTab="1" xr2:uid="{949A1E6F-A50E-0D47-B806-7BF7EBA35A5B}"/>
+    <workbookView xWindow="-35540" yWindow="900" windowWidth="29860" windowHeight="17240" activeTab="1" xr2:uid="{949A1E6F-A50E-0D47-B806-7BF7EBA35A5B}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="2" r:id="rId1"/>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1369" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1362" uniqueCount="421">
   <si>
     <t>table_name</t>
   </si>
@@ -963,9 +963,6 @@
     <t>wpcf-prgm_location</t>
   </si>
   <si>
-    <t>wpcf-prgm_k12_collaborate</t>
-  </si>
-  <si>
     <t>wpcf-prgm_conducted_outdoors</t>
   </si>
   <si>
@@ -1222,9 +1219,6 @@
   </si>
   <si>
     <t>Educator Fequency</t>
-  </si>
-  <si>
-    <t>K-12 Collaborate</t>
   </si>
   <si>
     <t>Conducted Outdoors</t>
@@ -2614,8 +2608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09851FDF-4334-4E44-81EF-4155DEF57BA3}">
   <dimension ref="A1:K122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A103" sqref="A103:XFD103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3529,7 +3523,7 @@
         <v>201</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D11" s="2">
         <v>3</v>
@@ -3561,7 +3555,7 @@
         <v>202</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D12" s="2">
         <v>12</v>
@@ -3625,7 +3619,7 @@
         <v>204</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D14" s="2">
         <v>14</v>
@@ -3657,7 +3651,7 @@
         <v>205</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D15" s="2">
         <v>15</v>
@@ -3689,7 +3683,7 @@
         <v>206</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D16" s="2">
         <v>16</v>
@@ -3721,7 +3715,7 @@
         <v>207</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D17" s="2">
         <v>2</v>
@@ -3753,7 +3747,7 @@
         <v>208</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D18" s="2">
         <v>17</v>
@@ -3788,7 +3782,7 @@
         <v>209</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="D19" s="2">
         <v>18</v>
@@ -3854,7 +3848,7 @@
         <v>212</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D21" s="2">
         <v>20</v>
@@ -3954,7 +3948,7 @@
         <v>214</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D24" s="2">
         <v>23</v>
@@ -3986,7 +3980,7 @@
         <v>215</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D25" s="2">
         <v>24</v>
@@ -4018,7 +4012,7 @@
         <v>216</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D26" s="2">
         <v>25</v>
@@ -4050,7 +4044,7 @@
         <v>217</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D27" s="2">
         <v>26</v>
@@ -4082,7 +4076,7 @@
         <v>218</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D28" s="2">
         <v>27</v>
@@ -4114,7 +4108,7 @@
         <v>219</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D29" s="2">
         <v>28</v>
@@ -4146,7 +4140,7 @@
         <v>220</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D30" s="2">
         <v>29</v>
@@ -4178,7 +4172,7 @@
         <v>221</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D31" s="2">
         <v>30</v>
@@ -4210,7 +4204,7 @@
         <v>222</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D32" s="2">
         <v>31</v>
@@ -4242,7 +4236,7 @@
         <v>223</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D33" s="2">
         <v>32</v>
@@ -4274,7 +4268,7 @@
         <v>224</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D34" s="2">
         <v>33</v>
@@ -4306,7 +4300,7 @@
         <v>225</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D35" s="2">
         <v>34</v>
@@ -4338,7 +4332,7 @@
         <v>226</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D36" s="2">
         <v>35</v>
@@ -4370,7 +4364,7 @@
         <v>227</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D37" s="2">
         <v>36</v>
@@ -4402,7 +4396,7 @@
         <v>228</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D38" s="2">
         <v>37</v>
@@ -4434,7 +4428,7 @@
         <v>229</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D39" s="2">
         <v>38</v>
@@ -4466,7 +4460,7 @@
         <v>230</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D40" s="2">
         <v>39</v>
@@ -4498,7 +4492,7 @@
         <v>231</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D41" s="2">
         <v>40</v>
@@ -4530,7 +4524,7 @@
         <v>232</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D42" s="2">
         <v>41</v>
@@ -4562,7 +4556,7 @@
         <v>233</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D43" s="2">
         <v>42</v>
@@ -4594,7 +4588,7 @@
         <v>234</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D44" s="2">
         <v>43</v>
@@ -4626,7 +4620,7 @@
         <v>235</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D45" s="2">
         <v>44</v>
@@ -4658,7 +4652,7 @@
         <v>236</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D46" s="2">
         <v>45</v>
@@ -4690,7 +4684,7 @@
         <v>237</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D47" s="2">
         <v>46</v>
@@ -4722,7 +4716,7 @@
         <v>238</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D48" s="2">
         <v>47</v>
@@ -4754,7 +4748,7 @@
         <v>239</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D49" s="2">
         <v>48</v>
@@ -4786,7 +4780,7 @@
         <v>240</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D50" s="2">
         <v>49</v>
@@ -4818,7 +4812,7 @@
         <v>241</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D51" s="2">
         <v>50</v>
@@ -4882,7 +4876,7 @@
         <v>243</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D53" s="2">
         <v>52</v>
@@ -4914,7 +4908,7 @@
         <v>244</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D54" s="2">
         <v>53</v>
@@ -4946,7 +4940,7 @@
         <v>245</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D55" s="2">
         <v>54</v>
@@ -4978,7 +4972,7 @@
         <v>246</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D56" s="2">
         <v>55</v>
@@ -5010,7 +5004,7 @@
         <v>247</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D57" s="2">
         <v>56</v>
@@ -5042,7 +5036,7 @@
         <v>248</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D58" s="2">
         <v>57</v>
@@ -5074,7 +5068,7 @@
         <v>249</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D59" s="2">
         <v>58</v>
@@ -5106,7 +5100,7 @@
         <v>250</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D60" s="2">
         <v>59</v>
@@ -5138,7 +5132,7 @@
         <v>251</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D61" s="2">
         <v>60</v>
@@ -5202,7 +5196,7 @@
         <v>253</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D63" s="2">
         <v>62</v>
@@ -5234,7 +5228,7 @@
         <v>254</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D64" s="2">
         <v>63</v>
@@ -5266,7 +5260,7 @@
         <v>255</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D65" s="2">
         <v>64</v>
@@ -5298,7 +5292,7 @@
         <v>256</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D66" s="2">
         <v>65</v>
@@ -5487,7 +5481,7 @@
         <v>30</v>
       </c>
       <c r="B72" s="19" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C72" s="8" t="s">
         <v>33</v>
@@ -5522,7 +5516,7 @@
         <v>257</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D73" s="2">
         <v>4</v>
@@ -5554,7 +5548,7 @@
         <v>258</v>
       </c>
       <c r="C74" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D74" s="4">
         <v>5</v>
@@ -5586,7 +5580,7 @@
         <v>259</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D75" s="2">
         <v>6</v>
@@ -5778,7 +5772,7 @@
         <v>260</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D81" s="2">
         <v>11</v>
@@ -5810,7 +5804,7 @@
         <v>261</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D82" s="4">
         <v>12</v>
@@ -5842,7 +5836,7 @@
         <v>262</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D83" s="2">
         <v>13</v>
@@ -5877,7 +5871,7 @@
         <v>263</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D84" s="4">
         <v>14</v>
@@ -5909,7 +5903,7 @@
         <v>268</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D85" s="2">
         <v>15</v>
@@ -5941,7 +5935,7 @@
         <v>269</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D86" s="4">
         <v>16</v>
@@ -5973,7 +5967,7 @@
         <v>266</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D87" s="2">
         <v>17</v>
@@ -6005,7 +5999,7 @@
         <v>267</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D88" s="4">
         <v>18</v>
@@ -6069,7 +6063,7 @@
         <v>271</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D90" s="4">
         <v>20</v>
@@ -6101,7 +6095,7 @@
         <v>272</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D91" s="2">
         <v>21</v>
@@ -6133,7 +6127,7 @@
         <v>273</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D92" s="4">
         <v>22</v>
@@ -6165,7 +6159,7 @@
         <v>274</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D93" s="2">
         <v>23</v>
@@ -6197,7 +6191,7 @@
         <v>275</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D94" s="4">
         <v>24</v>
@@ -6229,7 +6223,7 @@
         <v>276</v>
       </c>
       <c r="C95" s="17" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D95" s="2">
         <v>25</v>
@@ -6261,7 +6255,7 @@
         <v>277</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D96" s="4">
         <v>26</v>
@@ -6293,7 +6287,7 @@
         <v>278</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D97" s="2">
         <v>27</v>
@@ -6325,7 +6319,7 @@
         <v>281</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D98" s="4">
         <v>28</v>
@@ -6357,7 +6351,7 @@
         <v>282</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D99" s="2">
         <v>29</v>
@@ -6389,7 +6383,7 @@
         <v>283</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D100" s="4">
         <v>30</v>
@@ -6421,7 +6415,7 @@
         <v>284</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D101" s="2">
         <v>31</v>
@@ -6478,46 +6472,26 @@
       </c>
     </row>
     <row r="103" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B103" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="C103" s="2" t="s">
-        <v>373</v>
-      </c>
-      <c r="D103" s="2">
-        <v>33</v>
-      </c>
-      <c r="E103" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F103" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G103" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H103" s="2">
-        <v>0</v>
-      </c>
-      <c r="J103" s="2">
-        <v>0</v>
-      </c>
-      <c r="K103" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="A103" s="2"/>
+      <c r="B103" s="2"/>
+      <c r="C103" s="2"/>
+      <c r="D103" s="2"/>
+      <c r="E103" s="2"/>
+      <c r="F103" s="2"/>
+      <c r="G103" s="2"/>
+      <c r="H103" s="2"/>
+      <c r="J103" s="2"/>
+      <c r="K103" s="2"/>
     </row>
     <row r="104" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B104" s="14" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="D104" s="4">
         <v>34</v>
@@ -6546,10 +6520,10 @@
         <v>30</v>
       </c>
       <c r="B105" s="14" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D105" s="2">
         <v>35</v>
@@ -6578,10 +6552,10 @@
         <v>30</v>
       </c>
       <c r="B106" s="14" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="D106" s="4">
         <v>36</v>
@@ -6610,10 +6584,10 @@
         <v>30</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D107" s="2">
         <v>37</v>
@@ -6642,10 +6616,10 @@
         <v>30</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="D108" s="4">
         <v>38</v>
@@ -6674,10 +6648,10 @@
         <v>30</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D109" s="2">
         <v>39</v>
@@ -6706,10 +6680,10 @@
         <v>30</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D110" s="4">
         <v>40</v>
@@ -6738,10 +6712,10 @@
         <v>30</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D111" s="2">
         <v>41</v>
@@ -6770,7 +6744,7 @@
         <v>30</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C112" s="2" t="s">
         <v>96</v>
@@ -6802,10 +6776,10 @@
         <v>30</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="D113" s="2">
         <v>43</v>
@@ -6834,10 +6808,10 @@
         <v>30</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D114" s="4">
         <v>44</v>
@@ -6866,10 +6840,10 @@
         <v>30</v>
       </c>
       <c r="B115" s="18" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D115" s="2">
         <v>45</v>
@@ -6898,10 +6872,10 @@
         <v>30</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="D116" s="4">
         <v>46</v>
@@ -6930,10 +6904,10 @@
         <v>30</v>
       </c>
       <c r="B117" s="18" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D117" s="2">
         <v>47</v>
@@ -8362,10 +8336,10 @@
         <v>212</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="E47" s="2">
         <v>1</v>
@@ -8379,10 +8353,10 @@
         <v>212</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="E48" s="2">
         <v>2</v>
@@ -8396,10 +8370,10 @@
         <v>212</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="E49" s="2">
         <v>3</v>
@@ -8413,10 +8387,10 @@
         <v>212</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="E50" s="2">
         <v>4</v>
@@ -8430,10 +8404,10 @@
         <v>212</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="E51" s="2">
         <v>5</v>
@@ -8447,10 +8421,10 @@
         <v>212</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="E52" s="2">
         <v>6</v>
@@ -8464,10 +8438,10 @@
         <v>212</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="E53" s="2">
         <v>7</v>
@@ -9310,10 +9284,10 @@
         <v>260</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="E102" s="2">
         <v>1</v>
@@ -9327,10 +9301,10 @@
         <v>260</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="E103" s="2">
         <v>2</v>
@@ -9344,10 +9318,10 @@
         <v>260</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="E104" s="2">
         <v>3</v>
@@ -9361,10 +9335,10 @@
         <v>260</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="E105" s="2">
         <v>4</v>
@@ -9378,10 +9352,10 @@
         <v>260</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="E106" s="2">
         <v>5</v>
@@ -9395,10 +9369,10 @@
         <v>260</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="E107" s="2">
         <v>6</v>
@@ -9412,10 +9386,10 @@
         <v>260</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="E108" s="2">
         <v>7</v>
@@ -9429,10 +9403,10 @@
         <v>260</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="E109" s="2">
         <v>8</v>
@@ -9446,10 +9420,10 @@
         <v>260</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="E110" s="2">
         <v>9</v>
@@ -9463,10 +9437,10 @@
         <v>262</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="E111" s="2">
         <v>1</v>
@@ -9480,10 +9454,10 @@
         <v>262</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="E112" s="2">
         <v>2</v>
@@ -9497,10 +9471,10 @@
         <v>262</v>
       </c>
       <c r="C113" s="21" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D113" s="21" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="E113" s="2">
         <v>3</v>
@@ -9514,10 +9488,10 @@
         <v>262</v>
       </c>
       <c r="C114" s="21" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="D114" s="21" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="E114" s="2">
         <v>4</v>

</xml_diff>